<commit_message>
page version comparison and change highlighting in excel export
</commit_message>
<xml_diff>
--- a/templates/archive.xlsx
+++ b/templates/archive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbrandt/code/alexweb/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64C2BD9-C48D-DB4F-9A36-E85879CAEFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F6AED1-D55B-634F-9B7F-D12978099472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2260" yWindow="18000" windowWidth="41340" windowHeight="16160" xr2:uid="{F594BD6A-EF70-2449-B28F-2D0F86D4C3FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Comments</t>
   </si>
@@ -107,10 +107,22 @@
     <t>Archives / {id}</t>
   </si>
   <si>
-    <t>last changed:</t>
-  </si>
-  <si>
     <t>{col}</t>
+  </si>
+  <si>
+    <t>{edit:added}</t>
+  </si>
+  <si>
+    <t>{edit:changed}</t>
+  </si>
+  <si>
+    <t>{refmod}</t>
+  </si>
+  <si>
+    <t>ref. version:</t>
+  </si>
+  <si>
+    <t>version:</t>
   </si>
 </sst>
 </file>
@@ -203,7 +215,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +238,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE5E5E5"/>
         <bgColor rgb="FFE5E5E5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -297,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -394,6 +418,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,7 +763,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9:L9"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -837,7 +867,9 @@
       <c r="L3" s="4"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="O3" s="33" t="s">
+        <v>24</v>
+      </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -859,14 +891,17 @@
       <c r="A4" s="20"/>
       <c r="B4" s="16"/>
       <c r="C4" s="28" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="E4" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
@@ -874,7 +909,9 @@
       <c r="L4" s="17"/>
       <c r="M4" s="16"/>
       <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="O4" s="34" t="s">
+        <v>25</v>
+      </c>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
@@ -995,34 +1032,34 @@
         <v>19</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M7" s="30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>

</xml_diff>